<commit_message>
Main worker is RegExp; Rules update
</commit_message>
<xml_diff>
--- a/Programs/EXCEL/rules.xlsx
+++ b/Programs/EXCEL/rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\PycharmProjects\Data Analysing\EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D06911D-9071-4672-8401-415C45638631}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A96FAC8-877B-4BA6-A8F5-E83C9DEA4156}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Тип ТИ" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="292">
   <si>
     <t>A</t>
   </si>
@@ -859,25 +859,52 @@
     <t>_</t>
   </si>
   <si>
-    <t>\s[IU]a[^a-c]?</t>
-  </si>
-  <si>
-    <t>\s[IU]b[^a-c]?</t>
-  </si>
-  <si>
-    <t>\s[IU]c[^a-c]?</t>
-  </si>
-  <si>
-    <t>\s[IU]ab[^c]?</t>
-  </si>
-  <si>
-    <t>\s[IU]bc[^a]?</t>
-  </si>
-  <si>
-    <t>\s[IU]ac[^b]?</t>
-  </si>
-  <si>
-    <t>\s[IU]abc</t>
+    <t>\b[PQUI]a\b</t>
+  </si>
+  <si>
+    <t>\b[PQUI]b\b</t>
+  </si>
+  <si>
+    <t>\b[PQUI]c\b</t>
+  </si>
+  <si>
+    <t>\b[PQUI](a(?!a)|b(?!b)){2}\b</t>
+  </si>
+  <si>
+    <t>\b[PQUI](c(?!c)|b(?!b)){2}\b</t>
+  </si>
+  <si>
+    <t>\b[PQUI](a(?!a)|b(?!b)|c(?!c)){3}\b</t>
+  </si>
+  <si>
+    <t>\b[PQUI](a(?!a)|c(?!c)){2}\b</t>
+  </si>
+  <si>
+    <t>\bP[abc]?\b</t>
+  </si>
+  <si>
+    <t>\bQ[abc]?\b</t>
+  </si>
+  <si>
+    <t>\bU[abc]{0,3}\b</t>
+  </si>
+  <si>
+    <t>\bI[abc]{0,3}\b</t>
+  </si>
+  <si>
+    <t>\bF\b</t>
+  </si>
+  <si>
+    <t>\b(ШР|ТР|ЛР|ЗН)\b</t>
+  </si>
+  <si>
+    <t>^Земля\s+\d</t>
+  </si>
+  <si>
+    <t>^(МВ|В|СВ|СМВ)\b</t>
+  </si>
+  <si>
+    <t>\b(Срабатывание (защиты?|шкафа)|ДЗТ|ГЗТ|МТЗ|ДГЗ|ЗДЗ)\b</t>
   </si>
 </sst>
 </file>
@@ -1212,12 +1239,12 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="60" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1230,26 +1257,41 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>283</v>
+      </c>
       <c r="B2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>284</v>
+      </c>
       <c r="B3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>285</v>
+      </c>
       <c r="B4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>286</v>
+      </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>287</v>
+      </c>
       <c r="B6" t="s">
         <v>19</v>
       </c>
@@ -1449,13 +1491,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACBEDF88-AB50-4ECB-9A2D-30940E591FD7}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.44140625" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -1508,7 +1550,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -1516,7 +1558,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -1571,12 +1613,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31F442F7-CD06-464E-8817-937DD0B10CE7}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="55.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1609,6 +1652,9 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>288</v>
+      </c>
       <c r="B6" t="s">
         <v>63</v>
       </c>
@@ -1634,6 +1680,9 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>290</v>
+      </c>
       <c r="B11" t="s">
         <v>68</v>
       </c>
@@ -1663,82 +1712,88 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>291</v>
+      </c>
       <c r="B27" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>289</v>
+      </c>
       <c r="B31" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>89</v>
       </c>
@@ -1813,6 +1868,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="66" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2799,7 +2855,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>